<commit_message>
prépa routes méth atelier J2
</commit_message>
<xml_diff>
--- a/backend/docs/user_stories-and-routes.xlsx
+++ b/backend/docs/user_stories-and-routes.xlsx
@@ -564,18 +564,19 @@
   <dimension ref="A1:H65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="1" sqref="6:6 A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.6377551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.2397959183674"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.1479591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="56.1581632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="8.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.8826530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.7040816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="55.4795918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -683,6 +684,7 @@
       <c r="F6" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="G6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
@@ -697,6 +699,7 @@
       <c r="F7" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="G7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
@@ -711,6 +714,7 @@
       <c r="F8" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="G8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
@@ -725,6 +729,7 @@
       <c r="F9" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="G9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
@@ -739,6 +744,7 @@
       <c r="F10" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="G10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
@@ -756,6 +762,7 @@
       <c r="F11" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="G11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
@@ -767,6 +774,7 @@
       <c r="F12" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="G12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
@@ -781,6 +789,7 @@
       <c r="F13" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="G13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
@@ -792,6 +801,7 @@
       <c r="F14" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="G14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
@@ -919,19 +929,19 @@
   <dimension ref="A1:AB65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="6:6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="71.6734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="46.8418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="72.75"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="46.3010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="25.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
signupPost en cours de modif valid mail
</commit_message>
<xml_diff>
--- a/backend/docs/user_stories-and-routes.xlsx
+++ b/backend/docs/user_stories-and-routes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Stories" sheetId="1" state="visible" r:id="rId2"/>
@@ -374,7 +374,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -385,6 +385,24 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFEFEFEF"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99FF99"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66CCFF"/>
+        <bgColor rgb="FF33CCCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -435,13 +453,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -449,26 +475,94 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -529,9 +623,9 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FF99FF99"/>
       <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FF66CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
@@ -563,351 +657,394 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="1" sqref="6:6 A17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.8826530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.7040816326531"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="55.4795918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.9132653061224"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="49.515306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="51.1632653061225"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="54.8061224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="3" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+    <row r="2" s="11" customFormat="true" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="9"/>
+      <c r="E2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1" t="n">
+      <c r="F2" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="H2" s="10"/>
+    </row>
+    <row r="3" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="1" t="n">
+      <c r="E3" s="13"/>
+      <c r="F3" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="H3" s="10"/>
+    </row>
+    <row r="4" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="1" t="n">
+      <c r="E4" s="13"/>
+      <c r="F4" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="H4" s="10"/>
+    </row>
+    <row r="5" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="1" t="n">
+      <c r="E5" s="13"/>
+      <c r="F5" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="H5" s="10"/>
+    </row>
+    <row r="6" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="1" t="n">
+      <c r="E6" s="13"/>
+      <c r="F6" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="G6" s="0"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="1" t="n">
+      <c r="E7" s="13"/>
+      <c r="F7" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="G7" s="0"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="H7" s="10"/>
+    </row>
+    <row r="8" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="1" t="n">
+      <c r="E8" s="17"/>
+      <c r="F8" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="G8" s="0"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
+      <c r="H8" s="18"/>
+    </row>
+    <row r="9" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="1" t="n">
+      <c r="E9" s="17"/>
+      <c r="F9" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="G9" s="0"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
+      <c r="H9" s="18"/>
+    </row>
+    <row r="10" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="1" t="n">
+      <c r="E10" s="17"/>
+      <c r="F10" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="G10" s="0"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
+      <c r="H10" s="18"/>
+    </row>
+    <row r="11" s="16" customFormat="true" ht="24.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="1" t="n">
+      <c r="F11" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="G11" s="0"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
+      <c r="H11" s="18"/>
+    </row>
+    <row r="12" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="1" t="n">
+      <c r="C12" s="19"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="G12" s="0"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
+      <c r="H12" s="18"/>
+    </row>
+    <row r="13" s="16" customFormat="true" ht="24.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="1" t="n">
+      <c r="E13" s="15"/>
+      <c r="F13" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="G13" s="0"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
+      <c r="H13" s="18"/>
+    </row>
+    <row r="14" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="1" t="n">
+      <c r="C14" s="19"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="G14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
+      <c r="H14" s="18"/>
+    </row>
+    <row r="15" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="1" t="n">
+      <c r="C15" s="19"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="18" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
+      <c r="H15" s="18"/>
+    </row>
+    <row r="16" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="1" t="n">
+      <c r="E16" s="15"/>
+      <c r="F16" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="18" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
+      <c r="H16" s="18"/>
+    </row>
+    <row r="17" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="1" t="n">
+      <c r="C17" s="19"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="18" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
+      <c r="H17" s="18"/>
+    </row>
+    <row r="18" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="1" t="n">
+      <c r="E18" s="21"/>
+      <c r="F18" s="23" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+    </row>
+    <row r="19" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="1" t="n">
+      <c r="C19" s="24"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="23" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+    </row>
+    <row r="20" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="1" t="n">
+      <c r="C20" s="24"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="23" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+    </row>
+    <row r="21" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="F21" s="1" t="n">
+      <c r="C21" s="24"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="23" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+    </row>
+    <row r="22" s="22" customFormat="true" ht="27.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="F22" s="1" t="n">
+      <c r="E22" s="21"/>
+      <c r="F22" s="23" t="n">
         <v>3</v>
       </c>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -928,109 +1065,109 @@
   </sheetPr>
   <dimension ref="A1:AB65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="6:6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="72.75"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="46.3010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="71.8163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="45.7602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
-    <row r="1" s="8" customFormat="true" ht="25.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+    <row r="1" s="1" customFormat="true" ht="25.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
-      <c r="AA1" s="7"/>
-      <c r="AB1" s="7"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="27"/>
+      <c r="W1" s="27"/>
+      <c r="X1" s="27"/>
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="27"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="28" t="s">
         <v>58</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
+      <c r="U2" s="28"/>
+      <c r="V2" s="28"/>
+      <c r="W2" s="28"/>
+      <c r="X2" s="28"/>
+      <c r="Y2" s="28"/>
+      <c r="Z2" s="28"/>
+      <c r="AA2" s="28"/>
+      <c r="AB2" s="28"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -1056,7 +1193,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="30" t="s">
         <v>60</v>
       </c>
       <c r="B4" s="0" t="s">

</xml_diff>